<commit_message>
sửa báo cáo tổng hợp tiến độ
</commit_message>
<xml_diff>
--- a/EVN.Api/Templates/BaoCaoTongHopTienDo.xlsx
+++ b/EVN.Api/Templates/BaoCaoTongHopTienDo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeEvn\GiamSatTrungAp\GiamSatTrungAp_BE\EVN.Api\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87565DA9-EB07-4228-96B4-547138931350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B801B8-0BA9-4C8C-87BE-76AFB9756953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7CF2630E-7C15-40D4-B52D-67F942E1F7DD}"/>
   </bookViews>
@@ -378,8 +378,41 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -417,41 +450,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -828,7 +828,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,154 +845,154 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
     </row>
     <row r="2" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
     </row>
     <row r="3" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
     </row>
     <row r="5" spans="1:18" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="46" t="s">
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
     </row>
     <row r="6" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="25" t="s">
+      <c r="E7" s="37"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="28" t="s">
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="31" t="s">
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="33"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="44"/>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="23" t="s">
+      <c r="C8" s="35"/>
+      <c r="D8" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="34" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="5" t="s">
@@ -1001,38 +1001,38 @@
       <c r="H8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="31" t="s">
+      <c r="I8" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="33"/>
+      <c r="J8" s="44"/>
       <c r="K8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="31" t="s">
+      <c r="M8" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="33"/>
+      <c r="N8" s="44"/>
       <c r="O8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Q8" s="31" t="s">
+      <c r="Q8" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="R8" s="33"/>
+      <c r="R8" s="44"/>
     </row>
     <row r="9" spans="1:18" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5" t="s">
@@ -1319,7 +1319,7 @@
       <c r="R22" s="12"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
@@ -1339,7 +1339,7 @@
       <c r="R23" s="12"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
@@ -1359,7 +1359,7 @@
       <c r="R24" s="12"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
@@ -1379,7 +1379,7 @@
       <c r="R25" s="12"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
@@ -1399,7 +1399,7 @@
       <c r="R26" s="12"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="8"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
@@ -1419,7 +1419,7 @@
       <c r="R27" s="12"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
+      <c r="A28" s="8"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
@@ -1439,7 +1439,7 @@
       <c r="R28" s="12"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
+      <c r="A29" s="46"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
@@ -1459,7 +1459,7 @@
       <c r="R29" s="12"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
+      <c r="A30" s="46"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
@@ -1479,7 +1479,7 @@
       <c r="R30" s="12"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
+      <c r="A31" s="46"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
@@ -1499,7 +1499,7 @@
       <c r="R31" s="12"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
@@ -1519,7 +1519,7 @@
       <c r="R32" s="12"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
+      <c r="A33" s="8"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
@@ -1539,7 +1539,7 @@
       <c r="R33" s="12"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
+      <c r="A34" s="8"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
@@ -1559,7 +1559,7 @@
       <c r="R34" s="12"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
+      <c r="A35" s="8"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
@@ -1579,7 +1579,7 @@
       <c r="R35" s="12"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
+      <c r="A36" s="8"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
@@ -1599,7 +1599,7 @@
       <c r="R36" s="12"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
+      <c r="A37" s="8"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
@@ -1619,7 +1619,7 @@
       <c r="R37" s="12"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
+      <c r="A38" s="8"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
@@ -1639,7 +1639,7 @@
       <c r="R38" s="12"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
+      <c r="A39" s="8"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
@@ -1659,7 +1659,7 @@
       <c r="R39" s="12"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
+      <c r="A40" s="8"/>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
@@ -1679,7 +1679,7 @@
       <c r="R40" s="12"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
+      <c r="A41" s="8"/>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
@@ -1700,13 +1700,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="A3:P3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:F6"/>
-    <mergeCell ref="G5:R6"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="G7:J7"/>
@@ -1718,6 +1711,13 @@
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="A3:P3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:F6"/>
+    <mergeCell ref="G5:R6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>